<commit_message>
[ENH] pabi_account_special_project, adjust template
</commit_message>
<xml_diff>
--- a/pabi_account_special_project/xlsx_template/special_project.xlsx
+++ b/pabi_account_special_project/xlsx_template/special_project.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">Line Number</t>
   </si>
@@ -52,10 +52,7 @@
     <t xml:space="preserve">Credit</t>
   </si>
   <si>
-    <t xml:space="preserve">2018-10-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150930</t>
+    <t xml:space="preserve">20/05/2017</t>
   </si>
   <si>
     <t xml:space="preserve">TB_DECC_SEP 2015_2</t>
@@ -188,10 +185,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -327,23 +325,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,21 +433,21 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5465587044534"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.0971659919028"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="17.502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="13.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.4048582995951"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.3238866396761"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="18.6113360323887"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8947368421053"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,28 +457,28 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="ALG1" s="3"/>
@@ -516,28 +514,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>42885</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>100</v>
@@ -546,28 +544,28 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>42885</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="3" t="n">
@@ -576,28 +574,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>42885</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="3" t="n">
         <v>100</v>

</xml_diff>